<commit_message>
Change "Bauteil" to "Component" Change "bauteil" to "component"
</commit_message>
<xml_diff>
--- a/data/ExcelVorlage.xlsx
+++ b/data/ExcelVorlage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Masterarbeit\EXCEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\PycharmProjects\BIM-Excel-IFC-translater\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2E2CF8-96B1-4B6A-B603-DA3B383F85DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6290903C-8987-4C17-9EAE-33DCAE36E3D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{473C5BEC-D741-458D-94AD-63BB8E525707}"/>
+    <workbookView xWindow="0" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{473C5BEC-D741-458D-94AD-63BB8E525707}"/>
   </bookViews>
   <sheets>
     <sheet name="IfcWall" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Material</t>
   </si>
   <si>
-    <t>Bauteil</t>
-  </si>
-  <si>
     <t>Position [x,y,z]</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Glas</t>
+  </si>
+  <si>
+    <t>Component</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,19 +502,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -525,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -537,7 +537,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -577,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
@@ -597,7 +597,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -631,9 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1B6281-0DC8-4B97-9A5D-6ACA107A846B}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -642,19 +640,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -665,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4">
         <v>1.5</v>
@@ -677,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -685,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4">
         <v>1.5</v>
@@ -697,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +709,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,16 +719,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -741,7 +739,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4">
         <v>1.1000000000000001</v>
@@ -750,7 +748,7 @@
         <v>2.5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -758,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4">
         <v>1.1000000000000001</v>
@@ -767,7 +765,7 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change Excel Data "ExcelVorlage".
</commit_message>
<xml_diff>
--- a/data/ExcelVorlage.xlsx
+++ b/data/ExcelVorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\PycharmProjects\BIM-Excel-IFC-translater\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6290903C-8987-4C17-9EAE-33DCAE36E3D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2628F12B-D5A2-4E96-9ED6-38B399A272C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{473C5BEC-D741-458D-94AD-63BB8E525707}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{473C5BEC-D741-458D-94AD-63BB8E525707}"/>
   </bookViews>
   <sheets>
     <sheet name="IfcWall" sheetId="1" r:id="rId1"/>
@@ -33,69 +33,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
-  <si>
-    <t>WallCommon</t>
-  </si>
-  <si>
-    <t>WindowsCommon</t>
-  </si>
-  <si>
-    <t>DoorCommon</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Position [x,y,z]</t>
-  </si>
-  <si>
-    <t>0,0,0</t>
-  </si>
-  <si>
-    <t>0,5,0</t>
-  </si>
-  <si>
-    <t>5,5,0</t>
-  </si>
-  <si>
-    <t>5,0,0</t>
-  </si>
-  <si>
-    <t>Laenge [m]</t>
-  </si>
-  <si>
-    <t>Breite [m]</t>
-  </si>
-  <si>
-    <t>Hoehe [m]</t>
-  </si>
-  <si>
-    <t>Stahlbeton</t>
-  </si>
-  <si>
-    <t>Bruestungshoehe [m]</t>
-  </si>
-  <si>
-    <t>2,0,0</t>
-  </si>
-  <si>
-    <t>2,0,1</t>
-  </si>
-  <si>
-    <t>3,0,1</t>
-  </si>
-  <si>
-    <t>3,0,0</t>
-  </si>
-  <si>
-    <t>Holz</t>
-  </si>
-  <si>
-    <t>Glas</t>
-  </si>
-  <si>
-    <t>Component</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+  <si>
+    <t>COMPONENT</t>
+  </si>
+  <si>
+    <t>POSITION [x,y,z]</t>
+  </si>
+  <si>
+    <t>LENGTH [m]</t>
+  </si>
+  <si>
+    <t>DEPTH [m]</t>
+  </si>
+  <si>
+    <t>HEIGHT [m]</t>
+  </si>
+  <si>
+    <t>MATERIAL</t>
+  </si>
+  <si>
+    <t>reinforced concrete</t>
+  </si>
+  <si>
+    <t>concrete</t>
+  </si>
+  <si>
+    <t>masorny</t>
+  </si>
+  <si>
+    <t>VEKTOR [+-x/+-y]</t>
+  </si>
+  <si>
+    <t>+x</t>
+  </si>
+  <si>
+    <t>-x</t>
+  </si>
+  <si>
+    <t>+y</t>
+  </si>
+  <si>
+    <t>0;0;0</t>
+  </si>
+  <si>
+    <t>0;5;0</t>
+  </si>
+  <si>
+    <t>5;0;0</t>
+  </si>
+  <si>
+    <t>5;5;0</t>
+  </si>
+  <si>
+    <t>wall</t>
+  </si>
+  <si>
+    <t>wood</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>2;0;1</t>
+  </si>
+  <si>
+    <t>3;0;1</t>
+  </si>
+  <si>
+    <t>WIDTH [m]</t>
+  </si>
+  <si>
+    <t>glass</t>
+  </si>
+  <si>
+    <t>PARAPET HEIGHT [m]</t>
+  </si>
+  <si>
+    <t>3,50;0,00;0,00</t>
+  </si>
+  <si>
+    <t>3,00;0,00;0,00</t>
+  </si>
+  <si>
+    <t>door</t>
   </si>
 </sst>
 </file>
@@ -169,12 +190,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -489,137 +513,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C400C952-B6E2-481B-A18C-3E4799403395}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="5" customWidth="1"/>
+    <col min="4" max="6" width="20.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="6">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="6">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D5" s="6">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -631,71 +673,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1B6281-0DC8-4B97-9A5D-6ACA107A846B}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="20.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="6">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -709,42 +755,44 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>2.5</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -753,15 +801,15 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D3" s="4">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3" s="6">
         <v>2.5</v>
       </c>
       <c r="E3" s="2" t="s">

</xml_diff>